<commit_message>
Correcciones menores en modelo
</commit_message>
<xml_diff>
--- a/Diagramas/DiccDeDatos-final.xlsx
+++ b/Diagramas/DiccDeDatos-final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WINDOWS\Desktop\code\0-Taller\bdd-25\TPFinal-BaseDeDatos\Diagramas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C7CC92-6EC4-4D42-9775-1450C3AE4E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFB3D29-173E-47C1-8BC1-6CB939759DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="109">
   <si>
     <t>Usuario</t>
   </si>
@@ -353,12 +353,15 @@
   <si>
     <t>Marca(id)</t>
   </si>
+  <si>
+    <t>ciudad</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,6 +378,11 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -721,10 +729,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D118" sqref="D118"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1511,13 +1519,21 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="B23" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -1539,9 +1555,7 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="2"/>
       <c r="E24" s="1"/>
@@ -1569,27 +1583,15 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="B25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -1611,25 +1613,27 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H26" s="5"/>
+      <c r="B26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -1652,22 +1656,24 @@
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="5" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="F27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="5"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -1690,13 +1696,13 @@
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>11</v>
@@ -1704,7 +1710,7 @@
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -1727,13 +1733,23 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
+      <c r="B29" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -1755,9 +1771,7 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
       <c r="E30" s="1"/>
@@ -1785,27 +1799,15 @@
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="B31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
@@ -1827,25 +1829,27 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H32" s="5"/>
+      <c r="B32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -1868,19 +1872,23 @@
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="5" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D33" s="6"/>
+        <v>22</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E33" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G33" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="H33" s="5"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -1904,19 +1912,17 @@
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>50</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="D34" s="6"/>
       <c r="E34" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
@@ -1942,18 +1948,20 @@
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F35" s="5"/>
+      <c r="F35" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
       <c r="I35" s="1"/>
@@ -1978,13 +1986,13 @@
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>11</v>
@@ -2014,7 +2022,7 @@
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="5" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>9</v>
@@ -2027,9 +2035,7 @@
       </c>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
-      <c r="H37" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="H37" s="5"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
@@ -2052,13 +2058,13 @@
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>11</v>
@@ -2066,7 +2072,7 @@
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
@@ -2089,13 +2095,23 @@
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
+      <c r="B39" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
@@ -2117,9 +2133,7 @@
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
-      <c r="B40" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="2"/>
       <c r="E40" s="1"/>
@@ -2147,27 +2161,15 @@
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
-      <c r="B41" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="B41" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
@@ -2189,25 +2191,27 @@
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
-      <c r="B42" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H42" s="5"/>
+      <c r="B42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
@@ -2230,19 +2234,23 @@
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="5" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
+      <c r="F43" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="H43" s="5"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
@@ -2266,13 +2274,13 @@
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>11</v>
@@ -2302,20 +2310,18 @@
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F45" s="5">
-        <v>0</v>
-      </c>
+      <c r="F45" s="5"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
       <c r="I45" s="1"/>
@@ -2340,18 +2346,20 @@
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F46" s="5"/>
+      <c r="F46" s="5">
+        <v>0</v>
+      </c>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
       <c r="I46" s="1"/>
@@ -2376,22 +2384,20 @@
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
-      <c r="H47" s="5" t="s">
-        <v>64</v>
-      </c>
+      <c r="H47" s="5"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
@@ -2414,13 +2420,13 @@
     <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>11</v>
@@ -2428,7 +2434,7 @@
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
       <c r="H48" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
@@ -2451,13 +2457,23 @@
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
+      <c r="B49" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
@@ -2479,9 +2495,7 @@
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-      <c r="B50" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="2"/>
       <c r="E50" s="1"/>
@@ -2509,27 +2523,15 @@
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
-      <c r="B51" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="B51" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
@@ -2551,25 +2553,27 @@
     </row>
     <row r="52" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
-      <c r="B52" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H52" s="5"/>
+      <c r="B52" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
@@ -2592,19 +2596,23 @@
     <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="5" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D53" s="6"/>
+        <v>22</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E53" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G53" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="H53" s="5"/>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
@@ -2628,22 +2636,20 @@
     <row r="54" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="5" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>10</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="D54" s="6"/>
       <c r="E54" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F54" s="5"/>
+      <c r="F54" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="G54" s="5"/>
-      <c r="H54" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="H54" s="5"/>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
@@ -2665,13 +2671,23 @@
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
+      <c r="B55" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
@@ -2693,9 +2709,7 @@
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
-      <c r="B56" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -2723,27 +2737,15 @@
     </row>
     <row r="57" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
-      <c r="B57" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="B57" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
@@ -2765,25 +2767,27 @@
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
-      <c r="B58" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G58" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H58" s="5"/>
+      <c r="B58" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
@@ -2806,19 +2810,23 @@
     <row r="59" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="5" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5"/>
+      <c r="F59" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="H59" s="5"/>
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
@@ -2842,13 +2850,13 @@
     <row r="60" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="E60" s="5" t="s">
         <v>11</v>
@@ -2878,22 +2886,20 @@
     <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="5" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
-      <c r="H61" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="H61" s="5"/>
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
@@ -2916,7 +2922,7 @@
     <row r="62" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="5" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>22</v>
@@ -2930,7 +2936,7 @@
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
       <c r="H62" s="5" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
@@ -2953,13 +2959,23 @@
     </row>
     <row r="63" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
+      <c r="B63" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
@@ -2981,9 +2997,7 @@
     </row>
     <row r="64" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
-      <c r="B64" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="2"/>
       <c r="E64" s="1"/>
@@ -3011,27 +3025,15 @@
     </row>
     <row r="65" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
-      <c r="B65" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H65" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="B65" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C65" s="1"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
@@ -3053,25 +3055,27 @@
     </row>
     <row r="66" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
-      <c r="B66" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G66" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H66" s="5"/>
+      <c r="B66" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
@@ -3094,19 +3098,23 @@
     <row r="67" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="5" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D67" s="6"/>
+        <v>22</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E67" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G67" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="H67" s="5"/>
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
@@ -3130,22 +3138,20 @@
     <row r="68" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="5" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>10</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="D68" s="6"/>
       <c r="E68" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F68" s="5"/>
+      <c r="F68" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="G68" s="5"/>
-      <c r="H68" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="H68" s="5"/>
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
@@ -3168,13 +3174,13 @@
     <row r="69" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="5" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E69" s="5" t="s">
         <v>11</v>
@@ -3182,7 +3188,7 @@
       <c r="F69" s="5"/>
       <c r="G69" s="5"/>
       <c r="H69" s="5" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
@@ -3205,13 +3211,23 @@
     </row>
     <row r="70" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
+      <c r="B70" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5" t="s">
+        <v>74</v>
+      </c>
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
@@ -3233,9 +3249,7 @@
     </row>
     <row r="71" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
-      <c r="B71" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="2"/>
       <c r="E71" s="1"/>
@@ -3263,27 +3277,15 @@
     </row>
     <row r="72" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
-      <c r="B72" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F72" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G72" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H72" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="B72" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C72" s="1"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
@@ -3305,25 +3307,27 @@
     </row>
     <row r="73" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
-      <c r="B73" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G73" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H73" s="5"/>
+      <c r="B73" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H73" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
@@ -3346,19 +3350,23 @@
     <row r="74" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="5" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="E74" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
+      <c r="F74" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="H74" s="5"/>
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
@@ -3382,14 +3390,16 @@
     <row r="75" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D75" s="6"/>
+        <v>56</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>77</v>
+      </c>
       <c r="E75" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F75" s="5"/>
       <c r="G75" s="5"/>
@@ -3416,18 +3426,16 @@
     <row r="76" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="5" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="D76" s="6"/>
       <c r="E76" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>47</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F76" s="5"/>
       <c r="G76" s="5"/>
       <c r="H76" s="5"/>
       <c r="I76" s="1"/>
@@ -3452,22 +3460,20 @@
     <row r="77" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="5" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>10</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="D77" s="6"/>
       <c r="E77" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F77" s="5"/>
+      <c r="F77" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="G77" s="5"/>
-      <c r="H77" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="H77" s="5"/>
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
@@ -3490,13 +3496,13 @@
     <row r="78" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="5" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="E78" s="5" t="s">
         <v>11</v>
@@ -3504,7 +3510,7 @@
       <c r="F78" s="5"/>
       <c r="G78" s="5"/>
       <c r="H78" s="5" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
@@ -3527,13 +3533,23 @@
     </row>
     <row r="79" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
-      <c r="D79" s="2"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
-      <c r="G79" s="1"/>
-      <c r="H79" s="1"/>
+      <c r="B79" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
+      <c r="H79" s="5" t="s">
+        <v>74</v>
+      </c>
       <c r="I79" s="1"/>
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
@@ -3555,9 +3571,7 @@
     </row>
     <row r="80" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
-      <c r="B80" s="1" t="s">
-        <v>80</v>
-      </c>
+      <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="2"/>
       <c r="E80" s="1"/>
@@ -3585,27 +3599,15 @@
     </row>
     <row r="81" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
-      <c r="B81" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F81" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G81" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H81" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="B81" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C81" s="1"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
@@ -3627,25 +3629,27 @@
     </row>
     <row r="82" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
-      <c r="B82" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D82" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E82" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G82" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H82" s="5"/>
+      <c r="B82" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
@@ -3668,19 +3672,23 @@
     <row r="83" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="5" t="s">
-        <v>81</v>
+        <v>21</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>82</v>
+        <v>22</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>83</v>
+        <v>23</v>
       </c>
       <c r="E83" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F83" s="5"/>
-      <c r="G83" s="5"/>
+      <c r="F83" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="H83" s="5"/>
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
@@ -3704,13 +3712,13 @@
     <row r="84" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E84" s="5" t="s">
         <v>11</v>
@@ -3740,20 +3748,18 @@
     <row r="85" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="E85" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F85" s="5">
-        <v>0</v>
-      </c>
+      <c r="F85" s="5"/>
       <c r="G85" s="5"/>
       <c r="H85" s="5"/>
       <c r="I85" s="1"/>
@@ -3778,22 +3784,22 @@
     <row r="86" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="5" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E86" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F86" s="5"/>
+      <c r="F86" s="5">
+        <v>0</v>
+      </c>
       <c r="G86" s="5"/>
-      <c r="H86" s="5" t="s">
-        <v>74</v>
-      </c>
+      <c r="H86" s="5"/>
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
@@ -3816,13 +3822,13 @@
     <row r="87" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="5" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="C87" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>89</v>
+        <v>23</v>
       </c>
       <c r="E87" s="5" t="s">
         <v>11</v>
@@ -3830,7 +3836,7 @@
       <c r="F87" s="5"/>
       <c r="G87" s="5"/>
       <c r="H87" s="5" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="I87" s="1"/>
       <c r="J87" s="1"/>
@@ -3853,13 +3859,23 @@
     </row>
     <row r="88" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
-      <c r="C88" s="1"/>
-      <c r="D88" s="2"/>
-      <c r="E88" s="1"/>
-      <c r="F88" s="1"/>
-      <c r="G88" s="1"/>
-      <c r="H88" s="1"/>
+      <c r="B88" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F88" s="5"/>
+      <c r="G88" s="5"/>
+      <c r="H88" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="I88" s="1"/>
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
@@ -3881,9 +3897,7 @@
     </row>
     <row r="89" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
-      <c r="B89" s="1" t="s">
-        <v>91</v>
-      </c>
+      <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="2"/>
       <c r="E89" s="1"/>
@@ -3911,27 +3925,15 @@
     </row>
     <row r="90" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
-      <c r="B90" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D90" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F90" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G90" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H90" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="B90" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C90" s="1"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
+      <c r="H90" s="1"/>
       <c r="I90" s="1"/>
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
@@ -3953,25 +3955,27 @@
     </row>
     <row r="91" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
-      <c r="B91" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C91" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D91" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E91" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F91" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G91" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H91" s="5"/>
+      <c r="B91" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H91" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="I91" s="1"/>
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
@@ -3994,19 +3998,23 @@
     <row r="92" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="5" t="s">
-        <v>92</v>
+        <v>21</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E92" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F92" s="5"/>
-      <c r="G92" s="5"/>
+      <c r="F92" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G92" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="H92" s="5"/>
       <c r="I92" s="1"/>
       <c r="J92" s="1"/>
@@ -4030,13 +4038,13 @@
     <row r="93" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="5" t="s">
-        <v>52</v>
+        <v>92</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>93</v>
+        <v>9</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="E93" s="5" t="s">
         <v>11</v>
@@ -4065,13 +4073,21 @@
     </row>
     <row r="94" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
-      <c r="D94" s="2"/>
-      <c r="E94" s="1"/>
-      <c r="F94" s="1"/>
-      <c r="G94" s="1"/>
-      <c r="H94" s="1"/>
+      <c r="B94" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D94" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F94" s="5"/>
+      <c r="G94" s="5"/>
+      <c r="H94" s="5"/>
       <c r="I94" s="1"/>
       <c r="J94" s="1"/>
       <c r="K94" s="1"/>
@@ -4093,9 +4109,7 @@
     </row>
     <row r="95" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
-      <c r="B95" s="1" t="s">
-        <v>94</v>
-      </c>
+      <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="2"/>
       <c r="E95" s="1"/>
@@ -4123,27 +4137,15 @@
     </row>
     <row r="96" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
-      <c r="B96" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D96" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E96" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F96" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G96" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H96" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="B96" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C96" s="1"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
       <c r="I96" s="1"/>
       <c r="J96" s="1"/>
       <c r="K96" s="1"/>
@@ -4165,25 +4167,27 @@
     </row>
     <row r="97" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
-      <c r="B97" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C97" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D97" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E97" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F97" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G97" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H97" s="5"/>
+      <c r="B97" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H97" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="I97" s="1"/>
       <c r="J97" s="1"/>
       <c r="K97" s="1"/>
@@ -4206,19 +4210,23 @@
     <row r="98" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="E98" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F98" s="5"/>
-      <c r="G98" s="5"/>
+      <c r="F98" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G98" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="H98" s="5"/>
       <c r="I98" s="1"/>
       <c r="J98" s="1"/>
@@ -4242,13 +4250,13 @@
     <row r="99" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="5" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>95</v>
+        <v>14</v>
       </c>
       <c r="E99" s="5" t="s">
         <v>11</v>
@@ -4278,12 +4286,14 @@
     <row r="100" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="5" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D100" s="6"/>
+        <v>56</v>
+      </c>
+      <c r="D100" s="6" t="s">
+        <v>95</v>
+      </c>
       <c r="E100" s="5" t="s">
         <v>11</v>
       </c>
@@ -4312,14 +4322,12 @@
     <row r="101" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C101" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D101" s="6" t="s">
-        <v>98</v>
-      </c>
+      <c r="D101" s="6"/>
       <c r="E101" s="5" t="s">
         <v>11</v>
       </c>
@@ -4347,13 +4355,21 @@
     </row>
     <row r="102" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
-      <c r="D102" s="2"/>
-      <c r="E102" s="1"/>
-      <c r="F102" s="1"/>
-      <c r="G102" s="1"/>
-      <c r="H102" s="1"/>
+      <c r="B102" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D102" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F102" s="5"/>
+      <c r="G102" s="5"/>
+      <c r="H102" s="5"/>
       <c r="I102" s="1"/>
       <c r="J102" s="1"/>
       <c r="K102" s="1"/>
@@ -4375,9 +4391,7 @@
     </row>
     <row r="103" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
-      <c r="B103" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="2"/>
       <c r="E103" s="1"/>
@@ -4405,27 +4419,15 @@
     </row>
     <row r="104" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
-      <c r="B104" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D104" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F104" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G104" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H104" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="B104" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C104" s="1"/>
+      <c r="D104" s="2"/>
+      <c r="E104" s="1"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
       <c r="I104" s="1"/>
       <c r="J104" s="1"/>
       <c r="K104" s="1"/>
@@ -4447,25 +4449,27 @@
     </row>
     <row r="105" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
-      <c r="B105" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C105" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D105" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E105" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F105" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G105" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H105" s="5"/>
+      <c r="B105" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G105" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H105" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="I105" s="1"/>
       <c r="J105" s="1"/>
       <c r="K105" s="1"/>
@@ -4488,19 +4492,23 @@
     <row r="106" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="5" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D106" s="6"/>
+        <v>22</v>
+      </c>
+      <c r="D106" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E106" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F106" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="G106" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="G106" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="H106" s="5"/>
       <c r="I106" s="1"/>
       <c r="J106" s="1"/>
@@ -4524,22 +4532,20 @@
     <row r="107" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D107" s="6" t="s">
-        <v>23</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D107" s="6"/>
       <c r="E107" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F107" s="5"/>
+      <c r="F107" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="G107" s="5"/>
-      <c r="H107" s="5" t="s">
-        <v>104</v>
-      </c>
+      <c r="H107" s="5"/>
       <c r="I107" s="1"/>
       <c r="J107" s="1"/>
       <c r="K107" s="1"/>
@@ -4562,7 +4568,7 @@
     <row r="108" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="5" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="C108" s="5" t="s">
         <v>22</v>
@@ -4576,7 +4582,7 @@
       <c r="F108" s="5"/>
       <c r="G108" s="5"/>
       <c r="H108" s="5" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="I108" s="1"/>
       <c r="J108" s="1"/>
@@ -4599,13 +4605,23 @@
     </row>
     <row r="109" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
-      <c r="B109" s="1"/>
-      <c r="C109" s="1"/>
-      <c r="D109" s="2"/>
-      <c r="E109" s="1"/>
-      <c r="F109" s="1"/>
-      <c r="G109" s="1"/>
-      <c r="H109" s="1"/>
+      <c r="B109" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D109" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E109" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F109" s="5"/>
+      <c r="G109" s="5"/>
+      <c r="H109" s="5" t="s">
+        <v>74</v>
+      </c>
       <c r="I109" s="1"/>
       <c r="J109" s="1"/>
       <c r="K109" s="1"/>
@@ -4627,9 +4643,7 @@
     </row>
     <row r="110" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
-      <c r="B110" s="1" t="s">
-        <v>105</v>
-      </c>
+      <c r="B110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="2"/>
       <c r="E110" s="1"/>
@@ -4657,27 +4671,15 @@
     </row>
     <row r="111" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
-      <c r="B111" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D111" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E111" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F111" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G111" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H111" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="B111" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C111" s="1"/>
+      <c r="D111" s="2"/>
+      <c r="E111" s="1"/>
+      <c r="F111" s="1"/>
+      <c r="G111" s="1"/>
+      <c r="H111" s="1"/>
       <c r="I111" s="1"/>
       <c r="J111" s="1"/>
       <c r="K111" s="1"/>
@@ -4699,25 +4701,27 @@
     </row>
     <row r="112" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
-      <c r="B112" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C112" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D112" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E112" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F112" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G112" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H112" s="5"/>
+      <c r="B112" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G112" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H112" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="I112" s="1"/>
       <c r="J112" s="1"/>
       <c r="K112" s="1"/>
@@ -4739,21 +4743,25 @@
     </row>
     <row r="113" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
-      <c r="B113" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C113" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D113" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E113" s="13" t="s">
+      <c r="B113" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E113" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F113" s="13"/>
-      <c r="G113" s="13"/>
-      <c r="H113" s="13"/>
+      <c r="F113" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G113" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H113" s="5"/>
       <c r="I113" s="1"/>
       <c r="J113" s="1"/>
       <c r="K113" s="1"/>
@@ -4773,61 +4781,69 @@
       <c r="Y113" s="1"/>
       <c r="Z113" s="1"/>
     </row>
-    <row r="114" spans="1:26" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="10"/>
-      <c r="B114" s="10"/>
-      <c r="C114" s="10"/>
-      <c r="D114" s="11"/>
-      <c r="E114" s="10"/>
-      <c r="F114" s="10"/>
-      <c r="G114" s="10"/>
-      <c r="H114" s="10"/>
-      <c r="I114" s="10"/>
-      <c r="J114" s="10"/>
-      <c r="K114" s="10"/>
-      <c r="L114" s="10"/>
-      <c r="M114" s="10"/>
-      <c r="N114" s="10"/>
-      <c r="O114" s="10"/>
-      <c r="P114" s="10"/>
-      <c r="Q114" s="10"/>
-      <c r="R114" s="10"/>
-      <c r="S114" s="10"/>
-      <c r="T114" s="10"/>
-      <c r="U114" s="10"/>
-      <c r="V114" s="10"/>
-      <c r="W114" s="10"/>
-      <c r="X114" s="10"/>
-      <c r="Y114" s="10"/>
-      <c r="Z114" s="10"/>
-    </row>
-    <row r="115" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="1"/>
-      <c r="B115" s="1"/>
-      <c r="C115" s="1"/>
-      <c r="D115" s="2"/>
-      <c r="E115" s="1"/>
-      <c r="F115" s="1"/>
-      <c r="G115" s="1"/>
-      <c r="H115" s="1"/>
-      <c r="I115" s="1"/>
-      <c r="J115" s="1"/>
-      <c r="K115" s="1"/>
-      <c r="L115" s="1"/>
-      <c r="M115" s="1"/>
-      <c r="N115" s="1"/>
-      <c r="O115" s="1"/>
-      <c r="P115" s="1"/>
-      <c r="Q115" s="1"/>
-      <c r="R115" s="1"/>
-      <c r="S115" s="1"/>
-      <c r="T115" s="1"/>
-      <c r="U115" s="1"/>
-      <c r="V115" s="1"/>
-      <c r="W115" s="1"/>
-      <c r="X115" s="1"/>
-      <c r="Y115" s="1"/>
-      <c r="Z115" s="1"/>
+    <row r="114" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="1"/>
+      <c r="B114" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C114" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D114" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E114" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F114" s="13"/>
+      <c r="G114" s="13"/>
+      <c r="H114" s="13"/>
+      <c r="I114" s="1"/>
+      <c r="J114" s="1"/>
+      <c r="K114" s="1"/>
+      <c r="L114" s="1"/>
+      <c r="M114" s="1"/>
+      <c r="N114" s="1"/>
+      <c r="O114" s="1"/>
+      <c r="P114" s="1"/>
+      <c r="Q114" s="1"/>
+      <c r="R114" s="1"/>
+      <c r="S114" s="1"/>
+      <c r="T114" s="1"/>
+      <c r="U114" s="1"/>
+      <c r="V114" s="1"/>
+      <c r="W114" s="1"/>
+      <c r="X114" s="1"/>
+      <c r="Y114" s="1"/>
+      <c r="Z114" s="1"/>
+    </row>
+    <row r="115" spans="1:26" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="10"/>
+      <c r="B115" s="10"/>
+      <c r="C115" s="10"/>
+      <c r="D115" s="11"/>
+      <c r="E115" s="10"/>
+      <c r="F115" s="10"/>
+      <c r="G115" s="10"/>
+      <c r="H115" s="10"/>
+      <c r="I115" s="10"/>
+      <c r="J115" s="10"/>
+      <c r="K115" s="10"/>
+      <c r="L115" s="10"/>
+      <c r="M115" s="10"/>
+      <c r="N115" s="10"/>
+      <c r="O115" s="10"/>
+      <c r="P115" s="10"/>
+      <c r="Q115" s="10"/>
+      <c r="R115" s="10"/>
+      <c r="S115" s="10"/>
+      <c r="T115" s="10"/>
+      <c r="U115" s="10"/>
+      <c r="V115" s="10"/>
+      <c r="W115" s="10"/>
+      <c r="X115" s="10"/>
+      <c r="Y115" s="10"/>
+      <c r="Z115" s="10"/>
     </row>
     <row r="116" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
@@ -29637,7 +29653,36 @@
       <c r="Y1001" s="1"/>
       <c r="Z1001" s="1"/>
     </row>
+    <row r="1002" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1002" s="1"/>
+      <c r="B1002" s="1"/>
+      <c r="C1002" s="1"/>
+      <c r="D1002" s="2"/>
+      <c r="E1002" s="1"/>
+      <c r="F1002" s="1"/>
+      <c r="G1002" s="1"/>
+      <c r="H1002" s="1"/>
+      <c r="I1002" s="1"/>
+      <c r="J1002" s="1"/>
+      <c r="K1002" s="1"/>
+      <c r="L1002" s="1"/>
+      <c r="M1002" s="1"/>
+      <c r="N1002" s="1"/>
+      <c r="O1002" s="1"/>
+      <c r="P1002" s="1"/>
+      <c r="Q1002" s="1"/>
+      <c r="R1002" s="1"/>
+      <c r="S1002" s="1"/>
+      <c r="T1002" s="1"/>
+      <c r="U1002" s="1"/>
+      <c r="V1002" s="1"/>
+      <c r="W1002" s="1"/>
+      <c r="X1002" s="1"/>
+      <c r="Y1002" s="1"/>
+      <c r="Z1002" s="1"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup fitToHeight="0" orientation="portrait"/>
 </worksheet>

</xml_diff>